<commit_message>
updated code, fixed PER bug and added python ML code
</commit_message>
<xml_diff>
--- a/Resources/1991/Team_PER_1991.xlsx
+++ b/Resources/1991/Team_PER_1991.xlsx
@@ -22,85 +22,85 @@
     <t>PER</t>
   </si>
   <si>
+    <t>POR</t>
+  </si>
+  <si>
     <t>NJN</t>
   </si>
   <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>UTA</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>LAL</t>
+  </si>
+  <si>
+    <t>GSW</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
     <t>CHH</t>
   </si>
   <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>GSW</t>
-  </si>
-  <si>
-    <t>CLE</t>
-  </si>
-  <si>
-    <t>LAL</t>
-  </si>
-  <si>
-    <t>ATL</t>
-  </si>
-  <si>
-    <t>DET</t>
-  </si>
-  <si>
-    <t>POR</t>
+    <t>BOS</t>
   </si>
   <si>
     <t>WSB</t>
   </si>
   <si>
-    <t>PHI</t>
+    <t>SAC</t>
   </si>
   <si>
     <t>PHO</t>
   </si>
   <si>
-    <t>MIL</t>
-  </si>
-  <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>UTA</t>
+    <t>NYK</t>
   </si>
   <si>
     <t>MIN</t>
-  </si>
-  <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>SAS</t>
-  </si>
-  <si>
-    <t>HOU</t>
-  </si>
-  <si>
-    <t>NYK</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>SAC</t>
-  </si>
-  <si>
-    <t>LAC</t>
-  </si>
-  <si>
-    <t>BOS</t>
-  </si>
-  <si>
-    <t>ORL</t>
-  </si>
-  <si>
-    <t>MIA</t>
-  </si>
-  <si>
-    <t>IND</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>148.6</v>
+        <v>14.70909090909091</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -491,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>157.3</v>
+        <v>12.38333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,7 +502,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>143.1</v>
+        <v>12.95333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -513,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>173.3</v>
+        <v>15.12142857142857</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>194.3</v>
+        <v>12.15714285714286</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -535,7 +535,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>169.1</v>
+        <v>14.31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -546,7 +546,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>175.4</v>
+        <v>13.49230769230769</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>186</v>
+        <v>16.00833333333334</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -568,7 +568,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>161.8</v>
+        <v>11.88461538461539</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -579,7 +579,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>178.9</v>
+        <v>13.28571428571429</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -590,7 +590,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>153.4</v>
+        <v>12.35714285714286</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -601,7 +601,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>254.1</v>
+        <v>12.55384615384615</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -612,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>192.1</v>
+        <v>12.61428571428572</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -623,7 +623,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>179.5</v>
+        <v>13.63076923076923</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -634,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>176.6</v>
+        <v>12.82142857142857</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -645,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>173.2</v>
+        <v>14.09166666666667</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -656,7 +656,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>182.6</v>
+        <v>11.55333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -667,7 +667,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>173</v>
+        <v>13.31538461538462</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -678,7 +678,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>177.2</v>
+        <v>15.21666666666667</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -689,7 +689,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>175.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -700,7 +700,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>211.7</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -711,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>204</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -722,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>154.5</v>
+        <v>12.77857142857143</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -733,7 +733,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>211.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -744,7 +744,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>163.2</v>
+        <v>19.54615384615385</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -755,7 +755,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>170.2</v>
+        <v>12.55714285714286</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -766,7 +766,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>173.1</v>
+        <v>12.37142857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>